<commit_message>
split jobs to all multi-core
</commit_message>
<xml_diff>
--- a/scores_log.xlsx
+++ b/scores_log.xlsx
@@ -12,6 +12,11 @@
     <sheet name="gen_3" sheetId="3" r:id="rId3"/>
     <sheet name="gen_4" sheetId="4" r:id="rId4"/>
     <sheet name="gen_5" sheetId="5" r:id="rId5"/>
+    <sheet name="gen_6" sheetId="6" r:id="rId6"/>
+    <sheet name="gen_7" sheetId="7" r:id="rId7"/>
+    <sheet name="gen_8" sheetId="8" r:id="rId8"/>
+    <sheet name="gen_9" sheetId="9" r:id="rId9"/>
+    <sheet name="gen_10" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -465,6 +470,151 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1">
+        <v>78753245</v>
+      </c>
+      <c r="B1">
+        <v>719</v>
+      </c>
+      <c r="C1">
+        <v>1012814</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>79347187</v>
+      </c>
+      <c r="B2">
+        <v>726</v>
+      </c>
+      <c r="C2">
+        <v>1004568</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>78735928</v>
+      </c>
+      <c r="B3">
+        <v>718</v>
+      </c>
+      <c r="C3">
+        <v>1025312</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4">
+        <v>80212125</v>
+      </c>
+      <c r="B4">
+        <v>735</v>
+      </c>
+      <c r="C4">
+        <v>999094</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5">
+        <v>78753245</v>
+      </c>
+      <c r="B5">
+        <v>719</v>
+      </c>
+      <c r="C5">
+        <v>1014668</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6">
+        <v>79347187</v>
+      </c>
+      <c r="B6">
+        <v>726</v>
+      </c>
+      <c r="C6">
+        <v>1010156</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7">
+        <v>80404333</v>
+      </c>
+      <c r="B7">
+        <v>737</v>
+      </c>
+      <c r="C7">
+        <v>1002346</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8">
+        <v>80500437</v>
+      </c>
+      <c r="B8">
+        <v>738</v>
+      </c>
+      <c r="C8">
+        <v>1000280</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9">
+        <v>80884854</v>
+      </c>
+      <c r="B9">
+        <v>742</v>
+      </c>
+      <c r="C9">
+        <v>999792</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10">
+        <v>80404333</v>
+      </c>
+      <c r="B10">
+        <v>737</v>
+      </c>
+      <c r="C10">
+        <v>1002548</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11">
+        <v>79347187</v>
+      </c>
+      <c r="B11">
+        <v>726</v>
+      </c>
+      <c r="C11">
+        <v>1011388</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12">
+        <v>78753245</v>
+      </c>
+      <c r="B12">
+        <v>719</v>
+      </c>
+      <c r="C12">
+        <v>1016932</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C10"/>
@@ -966,4 +1116,606 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1">
+        <v>78735928</v>
+      </c>
+      <c r="B1">
+        <v>718</v>
+      </c>
+      <c r="C1">
+        <v>1025032</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>79347187</v>
+      </c>
+      <c r="B2">
+        <v>726</v>
+      </c>
+      <c r="C2">
+        <v>1011792</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>79058874</v>
+      </c>
+      <c r="B3">
+        <v>723</v>
+      </c>
+      <c r="C3">
+        <v>1021178</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4">
+        <v>80404333</v>
+      </c>
+      <c r="B4">
+        <v>737</v>
+      </c>
+      <c r="C4">
+        <v>1004100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5">
+        <v>80500437</v>
+      </c>
+      <c r="B5">
+        <v>738</v>
+      </c>
+      <c r="C5">
+        <v>1000280</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6">
+        <v>79058874</v>
+      </c>
+      <c r="B6">
+        <v>723</v>
+      </c>
+      <c r="C6">
+        <v>1024596</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7">
+        <v>79539395</v>
+      </c>
+      <c r="B7">
+        <v>728</v>
+      </c>
+      <c r="C7">
+        <v>1016192</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8">
+        <v>80212125</v>
+      </c>
+      <c r="B8">
+        <v>735</v>
+      </c>
+      <c r="C8">
+        <v>1015680</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9">
+        <v>80404333</v>
+      </c>
+      <c r="B9">
+        <v>737</v>
+      </c>
+      <c r="C9">
+        <v>1005114</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10">
+        <v>80884854</v>
+      </c>
+      <c r="B10">
+        <v>742</v>
+      </c>
+      <c r="C10">
+        <v>1000596</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1">
+        <v>78753245</v>
+      </c>
+      <c r="B1">
+        <v>719</v>
+      </c>
+      <c r="C1">
+        <v>1012814</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>78735928</v>
+      </c>
+      <c r="B2">
+        <v>718</v>
+      </c>
+      <c r="C2">
+        <v>1024760</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>79347187</v>
+      </c>
+      <c r="B3">
+        <v>726</v>
+      </c>
+      <c r="C3">
+        <v>1011472</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4">
+        <v>80404333</v>
+      </c>
+      <c r="B4">
+        <v>737</v>
+      </c>
+      <c r="C4">
+        <v>1002548</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5">
+        <v>80500437</v>
+      </c>
+      <c r="B5">
+        <v>738</v>
+      </c>
+      <c r="C5">
+        <v>1000280</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6">
+        <v>79539395</v>
+      </c>
+      <c r="B6">
+        <v>728</v>
+      </c>
+      <c r="C6">
+        <v>1015984</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7">
+        <v>79635499</v>
+      </c>
+      <c r="B7">
+        <v>729</v>
+      </c>
+      <c r="C7">
+        <v>1017564</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8">
+        <v>80212125</v>
+      </c>
+      <c r="B8">
+        <v>735</v>
+      </c>
+      <c r="C8">
+        <v>1015316</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9">
+        <v>79058874</v>
+      </c>
+      <c r="B9">
+        <v>723</v>
+      </c>
+      <c r="C9">
+        <v>1021164</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10">
+        <v>80404333</v>
+      </c>
+      <c r="B10">
+        <v>737</v>
+      </c>
+      <c r="C10">
+        <v>1004100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11">
+        <v>80884854</v>
+      </c>
+      <c r="B11">
+        <v>742</v>
+      </c>
+      <c r="C11">
+        <v>1000596</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1">
+        <v>78753245</v>
+      </c>
+      <c r="B1">
+        <v>719</v>
+      </c>
+      <c r="C1">
+        <v>1012814</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>78735928</v>
+      </c>
+      <c r="B2">
+        <v>718</v>
+      </c>
+      <c r="C2">
+        <v>1024776</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>79347187</v>
+      </c>
+      <c r="B3">
+        <v>726</v>
+      </c>
+      <c r="C3">
+        <v>1011388</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4">
+        <v>80404333</v>
+      </c>
+      <c r="B4">
+        <v>737</v>
+      </c>
+      <c r="C4">
+        <v>1002548</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5">
+        <v>80500437</v>
+      </c>
+      <c r="B5">
+        <v>738</v>
+      </c>
+      <c r="C5">
+        <v>1000280</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6">
+        <v>78753245</v>
+      </c>
+      <c r="B6">
+        <v>719</v>
+      </c>
+      <c r="C6">
+        <v>1016932</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7">
+        <v>79347187</v>
+      </c>
+      <c r="B7">
+        <v>726</v>
+      </c>
+      <c r="C7">
+        <v>1011472</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8">
+        <v>80884854</v>
+      </c>
+      <c r="B8">
+        <v>742</v>
+      </c>
+      <c r="C8">
+        <v>1000596</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9">
+        <v>80404333</v>
+      </c>
+      <c r="B9">
+        <v>737</v>
+      </c>
+      <c r="C9">
+        <v>1003960</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10">
+        <v>79539395</v>
+      </c>
+      <c r="B10">
+        <v>728</v>
+      </c>
+      <c r="C10">
+        <v>1015984</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11">
+        <v>80212125</v>
+      </c>
+      <c r="B11">
+        <v>735</v>
+      </c>
+      <c r="C11">
+        <v>1015316</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12">
+        <v>78753245</v>
+      </c>
+      <c r="B12">
+        <v>719</v>
+      </c>
+      <c r="C12">
+        <v>1024784</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13">
+        <v>80404333</v>
+      </c>
+      <c r="B13">
+        <v>737</v>
+      </c>
+      <c r="C13">
+        <v>1004100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1">
+        <v>78753245</v>
+      </c>
+      <c r="B1">
+        <v>719</v>
+      </c>
+      <c r="C1">
+        <v>1012814</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>80212125</v>
+      </c>
+      <c r="B2">
+        <v>735</v>
+      </c>
+      <c r="C2">
+        <v>999094</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>78735928</v>
+      </c>
+      <c r="B3">
+        <v>718</v>
+      </c>
+      <c r="C3">
+        <v>1024576</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4">
+        <v>79347187</v>
+      </c>
+      <c r="B4">
+        <v>726</v>
+      </c>
+      <c r="C4">
+        <v>1011388</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5">
+        <v>78753245</v>
+      </c>
+      <c r="B5">
+        <v>719</v>
+      </c>
+      <c r="C5">
+        <v>1016932</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6">
+        <v>79347187</v>
+      </c>
+      <c r="B6">
+        <v>726</v>
+      </c>
+      <c r="C6">
+        <v>1011472</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7">
+        <v>80404333</v>
+      </c>
+      <c r="B7">
+        <v>737</v>
+      </c>
+      <c r="C7">
+        <v>1002346</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8">
+        <v>80500437</v>
+      </c>
+      <c r="B8">
+        <v>738</v>
+      </c>
+      <c r="C8">
+        <v>1000280</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9">
+        <v>80884854</v>
+      </c>
+      <c r="B9">
+        <v>742</v>
+      </c>
+      <c r="C9">
+        <v>999792</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10">
+        <v>80596542</v>
+      </c>
+      <c r="B10">
+        <v>739</v>
+      </c>
+      <c r="C10">
+        <v>1001008</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11">
+        <v>79347187</v>
+      </c>
+      <c r="B11">
+        <v>726</v>
+      </c>
+      <c r="C11">
+        <v>1018020</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12">
+        <v>80212125</v>
+      </c>
+      <c r="B12">
+        <v>735</v>
+      </c>
+      <c r="C12">
+        <v>1015316</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13">
+        <v>80404333</v>
+      </c>
+      <c r="B13">
+        <v>737</v>
+      </c>
+      <c r="C13">
+        <v>1002548</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14">
+        <v>80308229</v>
+      </c>
+      <c r="B14">
+        <v>736</v>
+      </c>
+      <c r="C14">
+        <v>1011892</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15">
+        <v>79539395</v>
+      </c>
+      <c r="B15">
+        <v>728</v>
+      </c>
+      <c r="C15">
+        <v>1015984</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16">
+        <v>78753245</v>
+      </c>
+      <c r="B16">
+        <v>719</v>
+      </c>
+      <c r="C16">
+        <v>1023860</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
spread jobs to all cpu
</commit_message>
<xml_diff>
--- a/scores_log.xlsx
+++ b/scores_log.xlsx
@@ -12,11 +12,6 @@
     <sheet name="gen_3" sheetId="3" r:id="rId3"/>
     <sheet name="gen_4" sheetId="4" r:id="rId4"/>
     <sheet name="gen_5" sheetId="5" r:id="rId5"/>
-    <sheet name="gen_6" sheetId="6" r:id="rId6"/>
-    <sheet name="gen_7" sheetId="7" r:id="rId7"/>
-    <sheet name="gen_8" sheetId="8" r:id="rId8"/>
-    <sheet name="gen_9" sheetId="9" r:id="rId9"/>
-    <sheet name="gen_10" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -470,151 +465,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C12"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1">
-        <v>78753245</v>
-      </c>
-      <c r="B1">
-        <v>719</v>
-      </c>
-      <c r="C1">
-        <v>1012814</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2">
-        <v>79347187</v>
-      </c>
-      <c r="B2">
-        <v>726</v>
-      </c>
-      <c r="C2">
-        <v>1004568</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3">
-        <v>78735928</v>
-      </c>
-      <c r="B3">
-        <v>718</v>
-      </c>
-      <c r="C3">
-        <v>1025312</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4">
-        <v>80212125</v>
-      </c>
-      <c r="B4">
-        <v>735</v>
-      </c>
-      <c r="C4">
-        <v>999094</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5">
-        <v>78753245</v>
-      </c>
-      <c r="B5">
-        <v>719</v>
-      </c>
-      <c r="C5">
-        <v>1014668</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6">
-        <v>79347187</v>
-      </c>
-      <c r="B6">
-        <v>726</v>
-      </c>
-      <c r="C6">
-        <v>1010156</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7">
-        <v>80404333</v>
-      </c>
-      <c r="B7">
-        <v>737</v>
-      </c>
-      <c r="C7">
-        <v>1002346</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8">
-        <v>80500437</v>
-      </c>
-      <c r="B8">
-        <v>738</v>
-      </c>
-      <c r="C8">
-        <v>1000280</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9">
-        <v>80884854</v>
-      </c>
-      <c r="B9">
-        <v>742</v>
-      </c>
-      <c r="C9">
-        <v>999792</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10">
-        <v>80404333</v>
-      </c>
-      <c r="B10">
-        <v>737</v>
-      </c>
-      <c r="C10">
-        <v>1002548</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11">
-        <v>79347187</v>
-      </c>
-      <c r="B11">
-        <v>726</v>
-      </c>
-      <c r="C11">
-        <v>1011388</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12">
-        <v>78753245</v>
-      </c>
-      <c r="B12">
-        <v>719</v>
-      </c>
-      <c r="C12">
-        <v>1016932</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C10"/>
@@ -653,7 +503,7 @@
         <v>728</v>
       </c>
       <c r="C3">
-        <v>1022612</v>
+        <v>1023200</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -776,7 +626,7 @@
         <v>728</v>
       </c>
       <c r="C3">
-        <v>1018376</v>
+        <v>1019028</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -820,7 +670,7 @@
         <v>728</v>
       </c>
       <c r="C7">
-        <v>1022612</v>
+        <v>1023200</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -899,7 +749,7 @@
         <v>728</v>
       </c>
       <c r="C2">
-        <v>1016248</v>
+        <v>1016900</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -1022,7 +872,7 @@
         <v>728</v>
       </c>
       <c r="C2">
-        <v>1016192</v>
+        <v>1016844</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -1111,608 +961,6 @@
       </c>
       <c r="C10">
         <v>1000596</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1">
-        <v>78735928</v>
-      </c>
-      <c r="B1">
-        <v>718</v>
-      </c>
-      <c r="C1">
-        <v>1025032</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2">
-        <v>79347187</v>
-      </c>
-      <c r="B2">
-        <v>726</v>
-      </c>
-      <c r="C2">
-        <v>1011792</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3">
-        <v>79058874</v>
-      </c>
-      <c r="B3">
-        <v>723</v>
-      </c>
-      <c r="C3">
-        <v>1021178</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4">
-        <v>80404333</v>
-      </c>
-      <c r="B4">
-        <v>737</v>
-      </c>
-      <c r="C4">
-        <v>1004100</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5">
-        <v>80500437</v>
-      </c>
-      <c r="B5">
-        <v>738</v>
-      </c>
-      <c r="C5">
-        <v>1000280</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6">
-        <v>79058874</v>
-      </c>
-      <c r="B6">
-        <v>723</v>
-      </c>
-      <c r="C6">
-        <v>1024596</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7">
-        <v>79539395</v>
-      </c>
-      <c r="B7">
-        <v>728</v>
-      </c>
-      <c r="C7">
-        <v>1016192</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8">
-        <v>80212125</v>
-      </c>
-      <c r="B8">
-        <v>735</v>
-      </c>
-      <c r="C8">
-        <v>1015680</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9">
-        <v>80404333</v>
-      </c>
-      <c r="B9">
-        <v>737</v>
-      </c>
-      <c r="C9">
-        <v>1005114</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10">
-        <v>80884854</v>
-      </c>
-      <c r="B10">
-        <v>742</v>
-      </c>
-      <c r="C10">
-        <v>1000596</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1">
-        <v>78753245</v>
-      </c>
-      <c r="B1">
-        <v>719</v>
-      </c>
-      <c r="C1">
-        <v>1012814</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2">
-        <v>78735928</v>
-      </c>
-      <c r="B2">
-        <v>718</v>
-      </c>
-      <c r="C2">
-        <v>1024760</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3">
-        <v>79347187</v>
-      </c>
-      <c r="B3">
-        <v>726</v>
-      </c>
-      <c r="C3">
-        <v>1011472</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4">
-        <v>80404333</v>
-      </c>
-      <c r="B4">
-        <v>737</v>
-      </c>
-      <c r="C4">
-        <v>1002548</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5">
-        <v>80500437</v>
-      </c>
-      <c r="B5">
-        <v>738</v>
-      </c>
-      <c r="C5">
-        <v>1000280</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6">
-        <v>79539395</v>
-      </c>
-      <c r="B6">
-        <v>728</v>
-      </c>
-      <c r="C6">
-        <v>1015984</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7">
-        <v>79635499</v>
-      </c>
-      <c r="B7">
-        <v>729</v>
-      </c>
-      <c r="C7">
-        <v>1017564</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8">
-        <v>80212125</v>
-      </c>
-      <c r="B8">
-        <v>735</v>
-      </c>
-      <c r="C8">
-        <v>1015316</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9">
-        <v>79058874</v>
-      </c>
-      <c r="B9">
-        <v>723</v>
-      </c>
-      <c r="C9">
-        <v>1021164</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10">
-        <v>80404333</v>
-      </c>
-      <c r="B10">
-        <v>737</v>
-      </c>
-      <c r="C10">
-        <v>1004100</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11">
-        <v>80884854</v>
-      </c>
-      <c r="B11">
-        <v>742</v>
-      </c>
-      <c r="C11">
-        <v>1000596</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C13"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1">
-        <v>78753245</v>
-      </c>
-      <c r="B1">
-        <v>719</v>
-      </c>
-      <c r="C1">
-        <v>1012814</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2">
-        <v>78735928</v>
-      </c>
-      <c r="B2">
-        <v>718</v>
-      </c>
-      <c r="C2">
-        <v>1024776</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3">
-        <v>79347187</v>
-      </c>
-      <c r="B3">
-        <v>726</v>
-      </c>
-      <c r="C3">
-        <v>1011388</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4">
-        <v>80404333</v>
-      </c>
-      <c r="B4">
-        <v>737</v>
-      </c>
-      <c r="C4">
-        <v>1002548</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5">
-        <v>80500437</v>
-      </c>
-      <c r="B5">
-        <v>738</v>
-      </c>
-      <c r="C5">
-        <v>1000280</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6">
-        <v>78753245</v>
-      </c>
-      <c r="B6">
-        <v>719</v>
-      </c>
-      <c r="C6">
-        <v>1016932</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7">
-        <v>79347187</v>
-      </c>
-      <c r="B7">
-        <v>726</v>
-      </c>
-      <c r="C7">
-        <v>1011472</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8">
-        <v>80884854</v>
-      </c>
-      <c r="B8">
-        <v>742</v>
-      </c>
-      <c r="C8">
-        <v>1000596</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9">
-        <v>80404333</v>
-      </c>
-      <c r="B9">
-        <v>737</v>
-      </c>
-      <c r="C9">
-        <v>1003960</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10">
-        <v>79539395</v>
-      </c>
-      <c r="B10">
-        <v>728</v>
-      </c>
-      <c r="C10">
-        <v>1015984</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11">
-        <v>80212125</v>
-      </c>
-      <c r="B11">
-        <v>735</v>
-      </c>
-      <c r="C11">
-        <v>1015316</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12">
-        <v>78753245</v>
-      </c>
-      <c r="B12">
-        <v>719</v>
-      </c>
-      <c r="C12">
-        <v>1024784</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13">
-        <v>80404333</v>
-      </c>
-      <c r="B13">
-        <v>737</v>
-      </c>
-      <c r="C13">
-        <v>1004100</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C16"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1">
-        <v>78753245</v>
-      </c>
-      <c r="B1">
-        <v>719</v>
-      </c>
-      <c r="C1">
-        <v>1012814</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2">
-        <v>80212125</v>
-      </c>
-      <c r="B2">
-        <v>735</v>
-      </c>
-      <c r="C2">
-        <v>999094</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3">
-        <v>78735928</v>
-      </c>
-      <c r="B3">
-        <v>718</v>
-      </c>
-      <c r="C3">
-        <v>1024576</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4">
-        <v>79347187</v>
-      </c>
-      <c r="B4">
-        <v>726</v>
-      </c>
-      <c r="C4">
-        <v>1011388</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5">
-        <v>78753245</v>
-      </c>
-      <c r="B5">
-        <v>719</v>
-      </c>
-      <c r="C5">
-        <v>1016932</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6">
-        <v>79347187</v>
-      </c>
-      <c r="B6">
-        <v>726</v>
-      </c>
-      <c r="C6">
-        <v>1011472</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7">
-        <v>80404333</v>
-      </c>
-      <c r="B7">
-        <v>737</v>
-      </c>
-      <c r="C7">
-        <v>1002346</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8">
-        <v>80500437</v>
-      </c>
-      <c r="B8">
-        <v>738</v>
-      </c>
-      <c r="C8">
-        <v>1000280</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9">
-        <v>80884854</v>
-      </c>
-      <c r="B9">
-        <v>742</v>
-      </c>
-      <c r="C9">
-        <v>999792</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10">
-        <v>80596542</v>
-      </c>
-      <c r="B10">
-        <v>739</v>
-      </c>
-      <c r="C10">
-        <v>1001008</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11">
-        <v>79347187</v>
-      </c>
-      <c r="B11">
-        <v>726</v>
-      </c>
-      <c r="C11">
-        <v>1018020</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12">
-        <v>80212125</v>
-      </c>
-      <c r="B12">
-        <v>735</v>
-      </c>
-      <c r="C12">
-        <v>1015316</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13">
-        <v>80404333</v>
-      </c>
-      <c r="B13">
-        <v>737</v>
-      </c>
-      <c r="C13">
-        <v>1002548</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14">
-        <v>80308229</v>
-      </c>
-      <c r="B14">
-        <v>736</v>
-      </c>
-      <c r="C14">
-        <v>1011892</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15">
-        <v>79539395</v>
-      </c>
-      <c r="B15">
-        <v>728</v>
-      </c>
-      <c r="C15">
-        <v>1015984</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="A16">
-        <v>78753245</v>
-      </c>
-      <c r="B16">
-        <v>719</v>
-      </c>
-      <c r="C16">
-        <v>1023860</v>
       </c>
     </row>
   </sheetData>

</xml_diff>